<commit_message>
Created Final Document - Version.1 and also updated Glossary
</commit_message>
<xml_diff>
--- a/Glossary_Version.2.xlsx
+++ b/Glossary_Version.2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="70">
   <si>
     <t>Term</t>
   </si>
@@ -223,12 +223,36 @@
   <si>
     <t>varchar</t>
   </si>
+  <si>
+    <t>Room number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RN </t>
+  </si>
+  <si>
+    <t>Existing reservation</t>
+  </si>
+  <si>
+    <t>ER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CN </t>
+  </si>
+  <si>
+    <t>Confirmation Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AN </t>
+  </si>
+  <si>
+    <t>Availability Number</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,12 +275,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -265,8 +283,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="16"/>
+      <sz val="20"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -382,68 +413,91 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -725,374 +779,440 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="2" max="2" width="69.140625" customWidth="1"/>
-    <col min="3" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="28.140625" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" style="9" customWidth="1"/>
+    <col min="2" max="2" width="67.85546875" style="9" customWidth="1"/>
+    <col min="3" max="4" width="14" style="9" customWidth="1"/>
+    <col min="5" max="5" width="18" style="9" customWidth="1"/>
+    <col min="6" max="6" width="28.140625" style="9" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" style="9" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="18" t="s">
+    <row r="1" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="20"/>
-    </row>
-    <row r="3" spans="1:7" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="30"/>
+    </row>
+    <row r="3" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3" t="s">
+      <c r="C4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5" t="s">
+      <c r="C5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="1:7" s="17" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="G5" s="10"/>
+    </row>
+    <row r="6" spans="1:7" s="14" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6" t="s">
+      <c r="C6" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="13"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="17" customFormat="1" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="16"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-    </row>
-    <row r="8" spans="1:7" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
+    <row r="7" spans="1:7" s="14" customFormat="1" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="15"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+    </row>
+    <row r="8" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5" t="s">
+      <c r="C8" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
+    <row r="9" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5" t="s">
+      <c r="C9" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="5"/>
-    </row>
-    <row r="10" spans="1:7" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="10" t="s">
+      <c r="G9" s="10"/>
+    </row>
+    <row r="10" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5" t="s">
+      <c r="C10" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="5"/>
-    </row>
-    <row r="11" spans="1:7" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="10" t="s">
+      <c r="G10" s="10"/>
+    </row>
+    <row r="11" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5" t="s">
+      <c r="C11" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="5"/>
-    </row>
-    <row r="12" spans="1:7" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="10" t="s">
+      <c r="G11" s="10"/>
+    </row>
+    <row r="12" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5" t="s">
+      <c r="C12" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="10" t="s">
+    <row r="13" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="22" t="s">
         <v>28</v>
       </c>
       <c r="B13" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5" t="s">
+      <c r="C13" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="G13" s="5"/>
-    </row>
-    <row r="14" spans="1:7" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="10" t="s">
+      <c r="G13" s="10"/>
+    </row>
+    <row r="14" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5" t="s">
+      <c r="C14" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="G14" s="5"/>
-    </row>
-    <row r="15" spans="1:7" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="10" t="s">
+      <c r="G14" s="10"/>
+    </row>
+    <row r="15" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="17" t="s">
         <v>33</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5" t="s">
+      <c r="C15" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="G15" s="10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="10" t="s">
+    <row r="16" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="17" t="s">
         <v>37</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5" t="s">
+      <c r="C16" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="G16" s="5" t="s">
+      <c r="G16" s="10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="10" t="s">
+    <row r="17" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="17" t="s">
         <v>40</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5" t="s">
+      <c r="C17" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="G17" s="10" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="10" t="s">
+    <row r="18" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="17" t="s">
         <v>44</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5" t="s">
+      <c r="C18" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="G18" s="10" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="10" t="s">
+    <row r="19" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="17" t="s">
         <v>47</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5" t="s">
+      <c r="C19" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="G19" s="5"/>
-    </row>
-    <row r="20" spans="1:7" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="10" t="s">
+      <c r="G19" s="10"/>
+    </row>
+    <row r="20" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="17" t="s">
         <v>49</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5" t="s">
+      <c r="C20" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="G20" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="10" t="s">
+    <row r="21" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5" t="s">
+      <c r="C21" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" s="22"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="G21" s="5"/>
-    </row>
-    <row r="22" spans="1:7" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="G21" s="10"/>
+    </row>
+    <row r="22" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="25"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="25"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="20"/>
+    </row>
+    <row r="25" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="B26" s="25"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="18"/>
+    </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="G6:G7"/>
@@ -1104,6 +1224,6 @@
     <mergeCell ref="F6:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="67" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>